<commit_message>
Added User Account Cases
</commit_message>
<xml_diff>
--- a/code/src/test/Resources/SampleTestData/customer_sample_data.xlsx
+++ b/code/src/test/Resources/SampleTestData/customer_sample_data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -61,6 +61,12 @@
     <t xml:space="preserve">post_code</t>
   </si>
   <si>
+    <t xml:space="preserve">signin_title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">create_title</t>
+  </si>
+  <si>
     <t xml:space="preserve">vinayms</t>
   </si>
   <si>
@@ -82,7 +88,13 @@
     <t xml:space="preserve">IN</t>
   </si>
   <si>
-    <t xml:space="preserve">satish</t>
+    <t xml:space="preserve">Sign In with Email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create your account</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sanju</t>
   </si>
   <si>
     <t xml:space="preserve">satishd@gmail.com</t>
@@ -210,40 +222,40 @@
     </xf>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="*unknown*" xfId="20" builtinId="8"/>
   </cellStyles>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N5" activeCellId="0" sqref="N5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="1" style="1" width="8.81"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="1" style="1" width="8.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="12.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="9.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="8.81"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="8.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="11.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="10.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="1" width="8.81"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="10" style="1" width="8.81"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -283,28 +295,34 @@
       <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E2" s="1" t="n">
-        <v>9945723812</v>
+        <v>278439847</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H2" s="1" t="n">
         <v>1</v>
@@ -313,39 +331,45 @@
         <v>31</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="K2" s="2" t="n">
         <v>549</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="M2" s="1" t="n">
         <v>560070</v>
       </c>
+      <c r="N2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E3" s="1" t="n">
         <v>6360413814</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="H3" s="1" t="n">
         <v>0</v>
@@ -354,19 +378,25 @@
         <v>412</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="K3" s="1" t="n">
         <v>549</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="M3" s="1" t="n">
         <v>560021</v>
       </c>
+      <c r="N3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" display="asdf@1234"/>

</xml_diff>